<commit_message>
Game Skeloton BuyIn, Wager, Gameout Comes
</commit_message>
<xml_diff>
--- a/data/testData.xlsx
+++ b/data/testData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wdtablesys1-my.sharepoint.com/personal/prasad_kamble_wdtablesystems_com/Documents/Documents/PlayWrightProject/PlayWrightPOC/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wdtablesys1-my.sharepoint.com/personal/prasad_kamble_wdtablesys1_onmicrosoft_com/Documents/Documents/PlayWrightProject/PlayWrightPOC/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="63" documentId="11_F25DC773A252ABDACC1048D4E99B63705BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5DAFBF2F-937C-4F6B-908A-FDED83EE8FE0}"/>
+  <xr:revisionPtr revIDLastSave="141" documentId="11_F25DC773A252ABDACC1048D4E99B63705BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5401DCA-7CD5-4080-8372-8DD452B985C1}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t>testCase_ID</t>
   </si>
@@ -63,15 +63,9 @@
     <t>TEST-0608</t>
   </si>
   <si>
-    <t>100;Rated-6009;1</t>
-  </si>
-  <si>
     <t>buyIn1(Denom-Count; Type-Id; Seat)</t>
   </si>
   <si>
-    <t>100;P1</t>
-  </si>
-  <si>
     <t>2s</t>
   </si>
   <si>
@@ -79,16 +73,88 @@
   </si>
   <si>
     <t>3s</t>
+  </si>
+  <si>
+    <t>P1;100;P1</t>
+  </si>
+  <si>
+    <t>100;rated-6009;1</t>
+  </si>
+  <si>
+    <t>buyIn2</t>
+  </si>
+  <si>
+    <t>wager2</t>
+  </si>
+  <si>
+    <t>wager3</t>
+  </si>
+  <si>
+    <t>wager4</t>
+  </si>
+  <si>
+    <t>buyIn3</t>
+  </si>
+  <si>
+    <t>100;anon</t>
+  </si>
+  <si>
+    <t>buyIn4</t>
+  </si>
+  <si>
+    <t>buyIn5</t>
+  </si>
+  <si>
+    <t>buyIn6</t>
+  </si>
+  <si>
+    <t>100;known-6010</t>
+  </si>
+  <si>
+    <t>100;known-6012</t>
+  </si>
+  <si>
+    <t>wager5</t>
+  </si>
+  <si>
+    <t>wager6</t>
+  </si>
+  <si>
+    <t>P2;100;P2</t>
+  </si>
+  <si>
+    <t>buyIn7</t>
+  </si>
+  <si>
+    <t>wager7</t>
+  </si>
+  <si>
+    <t>P5;100;P6</t>
+  </si>
+  <si>
+    <t>P3;100;B3</t>
+  </si>
+  <si>
+    <t>P4;100;B5</t>
+  </si>
+  <si>
+    <t>100;rated-6004;3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -396,84 +462,148 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="9" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="29.7109375" customWidth="1"/>
+    <col min="9" max="9" width="24" bestFit="1" customWidth="1"/>
+    <col min="10" max="15" width="24" customWidth="1"/>
+    <col min="16" max="21" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="J1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="Q1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="R1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="S1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="T1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="U1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="V1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="W1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="X1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M2" t="s">
+        <v>34</v>
+      </c>
+      <c r="P2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" t="s">
+      <c r="R2" t="s">
         <v>15</v>
       </c>
-      <c r="E2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" t="s">
-        <v>16</v>
+      <c r="S2" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Add the Payouts take Logic
</commit_message>
<xml_diff>
--- a/data/testData.xlsx
+++ b/data/testData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wdtablesys1-my.sharepoint.com/personal/prasad_kamble_wdtablesys1_onmicrosoft_com/Documents/Documents/PlayWrightProject/PlayWrightPOC/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="141" documentId="11_F25DC773A252ABDACC1048D4E99B63705BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5401DCA-7CD5-4080-8372-8DD452B985C1}"/>
+  <xr:revisionPtr revIDLastSave="156" documentId="11_F25DC773A252ABDACC1048D4E99B63705BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4EF81902-BF5D-450B-A234-91161035C1D1}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
   <si>
     <t>testCase_ID</t>
   </si>
@@ -51,9 +51,6 @@
     <t>card6</t>
   </si>
   <si>
-    <t>payAmt1;Antenna;Player</t>
-  </si>
-  <si>
     <t>payAmt2</t>
   </si>
   <si>
@@ -139,6 +136,24 @@
   </si>
   <si>
     <t>100;rated-6004;3</t>
+  </si>
+  <si>
+    <t>TakeBets</t>
+  </si>
+  <si>
+    <t>B3;B5</t>
+  </si>
+  <si>
+    <t>P1;100</t>
+  </si>
+  <si>
+    <t>P2;100</t>
+  </si>
+  <si>
+    <t>P6;100</t>
+  </si>
+  <si>
+    <t>payAmt1;Antenna</t>
   </si>
 </sst>
 </file>
@@ -462,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X2"/>
+  <dimension ref="A1:Y2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="W1" sqref="W1:Y2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,55 +492,56 @@
     <col min="9" max="9" width="24" bestFit="1" customWidth="1"/>
     <col min="10" max="15" width="24" customWidth="1"/>
     <col min="16" max="21" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
         <v>24</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>25</v>
       </c>
-      <c r="G1" t="s">
-        <v>26</v>
-      </c>
       <c r="H1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I1" t="s">
         <v>1</v>
       </c>
       <c r="J1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" t="s">
         <v>19</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>20</v>
       </c>
-      <c r="L1" t="s">
-        <v>21</v>
-      </c>
       <c r="M1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N1" t="s">
         <v>29</v>
       </c>
-      <c r="N1" t="s">
-        <v>30</v>
-      </c>
       <c r="O1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="P1" t="s">
         <v>2</v>
@@ -546,60 +562,75 @@
         <v>7</v>
       </c>
       <c r="V1" t="s">
+        <v>37</v>
+      </c>
+      <c r="W1" t="s">
+        <v>42</v>
+      </c>
+      <c r="X1" t="s">
         <v>8</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>9</v>
       </c>
-      <c r="X1" t="s">
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" t="s">
         <v>27</v>
       </c>
-      <c r="D2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2" t="s">
-        <v>28</v>
-      </c>
       <c r="I2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K2" t="s">
+        <v>34</v>
+      </c>
+      <c r="L2" t="s">
         <v>35</v>
       </c>
-      <c r="L2" t="s">
-        <v>36</v>
-      </c>
       <c r="M2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="P2" t="s">
         <v>13</v>
       </c>
       <c r="Q2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="R2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="S2" t="s">
         <v>14</v>
+      </c>
+      <c r="V2" t="s">
+        <v>38</v>
+      </c>
+      <c r="W2" t="s">
+        <v>39</v>
+      </c>
+      <c r="X2" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
3 Test Case Complete
</commit_message>
<xml_diff>
--- a/data/testData.xlsx
+++ b/data/testData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wdtablesys1-my.sharepoint.com/personal/prasad_kamble_wdtablesys1_onmicrosoft_com/Documents/Documents/PlayWrightProject/PlayWrightPOC/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="176" documentId="11_F25DC773A252ABDACC1048D4E99B63705BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6987A918-F762-4F59-A590-18CB3CE57753}"/>
+  <xr:revisionPtr revIDLastSave="208" documentId="11_F25DC773A252ABDACC1048D4E99B63705BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B75B0A27-BD6F-4DF4-9FDD-1EDB9205A99A}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="45">
   <si>
     <t>testCase_ID</t>
   </si>
@@ -127,6 +127,39 @@
   </si>
   <si>
     <t>B5;TGT</t>
+  </si>
+  <si>
+    <t>TEST-28845</t>
+  </si>
+  <si>
+    <t>100;rated-6009;1</t>
+  </si>
+  <si>
+    <t>P1;100;P1</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>TEST-14007</t>
+  </si>
+  <si>
+    <t>1000-2;anon</t>
+  </si>
+  <si>
+    <t>P1;1000;B3</t>
+  </si>
+  <si>
+    <t>P1;1000;P2</t>
+  </si>
+  <si>
+    <t>4s</t>
+  </si>
+  <si>
+    <t>Ah</t>
+  </si>
+  <si>
+    <t>B3;P2</t>
   </si>
 </sst>
 </file>
@@ -450,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y2"/>
+  <dimension ref="A1:Y4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="Y8" sqref="Y8"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="V7" sqref="V7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,6 +612,61 @@
         <v>33</v>
       </c>
     </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" t="s">
+        <v>36</v>
+      </c>
+      <c r="P3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>13</v>
+      </c>
+      <c r="R3" t="s">
+        <v>14</v>
+      </c>
+      <c r="S3" t="s">
+        <v>13</v>
+      </c>
+      <c r="V3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I4" t="s">
+        <v>40</v>
+      </c>
+      <c r="J4" t="s">
+        <v>41</v>
+      </c>
+      <c r="P4" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>42</v>
+      </c>
+      <c r="R4" t="s">
+        <v>12</v>
+      </c>
+      <c r="S4" t="s">
+        <v>43</v>
+      </c>
+      <c r="V4" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Developed Test cases of Table UI
</commit_message>
<xml_diff>
--- a/data/testData.xlsx
+++ b/data/testData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wdtablesystems-my.sharepoint.com/personal/prasad_kamble_wdtablesystems_com/Documents/Documents/PlayWrightProject/PlayWright_POC/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wdtablesystems-my.sharepoint.com/personal/vishal_khurana_wdtablesystems_com/Documents/PlayWright_Project/PlayWright_POC/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="220" documentId="11_F25DC773A252ABDACC1048D4E99B63705BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6341E1FE-0DD6-411C-974F-69D09C88A2F2}"/>
+  <xr:revisionPtr revIDLastSave="225" documentId="11_F25DC773A252ABDACC1048D4E99B63705BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D5629A3F-DBC2-436B-8E67-7DB99790BA67}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="testData" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
   <si>
     <t>testCase_ID</t>
   </si>
@@ -163,6 +163,12 @@
   </si>
   <si>
     <t>TEST-1999</t>
+  </si>
+  <si>
+    <t>TEST-34227</t>
+  </si>
+  <si>
+    <t>TEST-34229</t>
   </si>
 </sst>
 </file>
@@ -486,27 +492,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y5"/>
+  <dimension ref="A1:Y7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="29.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="29.7265625" customWidth="1"/>
     <col min="9" max="9" width="24" bestFit="1" customWidth="1"/>
     <col min="10" max="15" width="24" customWidth="1"/>
-    <col min="16" max="21" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="21" width="5.7265625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="9" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="23.54296875" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="8.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -583,7 +589,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -615,7 +621,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -641,7 +647,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -670,9 +676,19 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>